<commit_message>
changed Norway status and trend for AO so that it only reflects FIS part of the score - sea ice is now NA. Sea Ice not deemed a relevant part of artisinal opportunities in Norway.
</commit_message>
<xml_diff>
--- a/circle2016/prep/AO/combined_scores.xlsx
+++ b/circle2016/prep/AO/combined_scores.xlsx
@@ -13,7 +13,11 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$D$49</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="10">
   <si>
     <t>region_id</t>
   </si>
@@ -408,7 +412,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1105,4 +1109,706 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>73</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>47.5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>90.6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>92.9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>22.4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>-2.8999999999999998E-3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>5.2699999999999997E-2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>-4.7999999999999996E-3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>-7.8399999999999997E-2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <v>6.9099999999999995E-2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <v>1.8700000000000001E-2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>89</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>80.833333330000002</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>81.25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>82.5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>100</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>76</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>80</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>-1.4500000000000001E-2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27">
+        <v>-2.8E-3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28">
+        <v>3.2899999999999999E-2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29">
+        <v>-1.06E-2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>8</v>
+      </c>
+      <c r="B32">
+        <v>2.1299999999999999E-2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <v>-1.09E-2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <v>85.556666969779599</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>2</v>
+      </c>
+      <c r="B35">
+        <v>98.485324354995996</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>3</v>
+      </c>
+      <c r="B36">
+        <v>95.977377858415494</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>4</v>
+      </c>
+      <c r="B37">
+        <v>88.808763100682398</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>5</v>
+      </c>
+      <c r="B38">
+        <v>60.629391995111497</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>6</v>
+      </c>
+      <c r="B39">
+        <v>38.383838383838402</v>
+      </c>
+      <c r="C39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>8</v>
+      </c>
+      <c r="B40">
+        <v>84.403566506342699</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>9</v>
+      </c>
+      <c r="B41">
+        <v>94.184590872880406</v>
+      </c>
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42">
+        <v>1.6522423288748998E-2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>2</v>
+      </c>
+      <c r="B43">
+        <v>3.0687124749834E-2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>3</v>
+      </c>
+      <c r="B44">
+        <v>6.21479899009535E-2</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>4</v>
+      </c>
+      <c r="B45">
+        <v>1.6521990740741399E-2</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>5</v>
+      </c>
+      <c r="B46">
+        <v>-0.25945470536499698</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>6</v>
+      </c>
+      <c r="B47">
+        <v>-0.40000000000000502</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>8</v>
+      </c>
+      <c r="B48">
+        <v>6.7917956656348505E-2</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>9</v>
+      </c>
+      <c r="B49">
+        <v>-8.3393763596813497E-3</v>
+      </c>
+      <c r="C49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D49"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update layers.csv with new AO scores from changes to ao_fis
</commit_message>
<xml_diff>
--- a/circle2016/prep/AO/combined_scores.xlsx
+++ b/circle2016/prep/AO/combined_scores.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9108"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9108" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="11">
   <si>
     <t>region_id</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>overall scores</t>
   </si>
 </sst>
 </file>
@@ -411,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -439,7 +442,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>45</v>
+        <v>45.8</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -453,7 +456,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>73</v>
+        <v>78.5</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -481,7 +484,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>19</v>
+        <v>35.1</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -509,7 +512,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>90.6</v>
+        <v>99.6</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -523,7 +526,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>92.9</v>
+        <v>96.7</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -537,7 +540,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>22.4</v>
+        <v>43.3</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -551,7 +554,7 @@
         <v>1</v>
       </c>
       <c r="B10">
-        <v>-2.8999999999999998E-3</v>
+        <v>-3.0999999999999999E-3</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -565,7 +568,7 @@
         <v>2</v>
       </c>
       <c r="B11">
-        <v>5.2699999999999997E-2</v>
+        <v>-7.6E-3</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -579,7 +582,7 @@
         <v>3</v>
       </c>
       <c r="B12">
-        <v>-4.7999999999999996E-3</v>
+        <v>-4.8999999999999998E-3</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -593,7 +596,7 @@
         <v>4</v>
       </c>
       <c r="B13">
-        <v>-7.8399999999999997E-2</v>
+        <v>-6.59E-2</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
@@ -621,7 +624,7 @@
         <v>6</v>
       </c>
       <c r="B15">
-        <v>6.9099999999999995E-2</v>
+        <v>-1E-3</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
@@ -635,7 +638,7 @@
         <v>8</v>
       </c>
       <c r="B16">
-        <v>0.13930000000000001</v>
+        <v>-2.0999999999999999E-3</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
@@ -649,7 +652,7 @@
         <v>9</v>
       </c>
       <c r="B17">
-        <v>1.8700000000000001E-2</v>
+        <v>-6.9699999999999998E-2</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
@@ -1113,15 +1116,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1134,13 +1140,16 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>45</v>
+        <v>45.8</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1148,13 +1157,17 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <f>SUM(B2+B18+B34)/3</f>
+        <v>73.452222323259875</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>73</v>
+        <v>78.5</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -1162,8 +1175,12 @@
       <c r="D3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <f t="shared" ref="E3:E22" si="0">SUM(B3+B19+B35)/3</f>
+        <v>85.939552561665337</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1176,13 +1193,17 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>74.909125952805155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>19</v>
+        <v>35.1</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -1190,8 +1211,12 @@
       <c r="D5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>68.802921033560793</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1204,13 +1229,17 @@
       <c r="D6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <f>SUM(B22+B38)/2</f>
+        <v>80.314695997555745</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>90.6</v>
+        <v>99.6</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -1218,13 +1247,17 @@
       <c r="D7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <f>B7</f>
+        <v>99.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
       <c r="B8">
-        <v>92.9</v>
+        <v>96.7</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -1232,13 +1265,17 @@
       <c r="D8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>85.701188835447567</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>22.4</v>
+        <v>43.3</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -1246,13 +1283,17 @@
       <c r="D9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>72.494863624293473</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10">
-        <v>-2.8999999999999998E-3</v>
+        <v>-3.0999999999999999E-3</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -1260,13 +1301,17 @@
       <c r="D10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>-3.5919223708366757E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
       <c r="B11">
-        <v>5.2699999999999997E-2</v>
+        <v>-7.6E-3</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -1274,13 +1319,17 @@
       <c r="D11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <f>SUM(B11+B27+B43)/3</f>
+        <v>6.7623749166113335E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
       <c r="B12">
-        <v>-4.7999999999999996E-3</v>
+        <v>-4.8999999999999998E-3</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -1288,13 +1337,17 @@
       <c r="D12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>3.0049329966984496E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>4</v>
       </c>
       <c r="B13">
-        <v>-7.8399999999999997E-2</v>
+        <v>-6.59E-2</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
@@ -1302,8 +1355,12 @@
       <c r="D13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>-1.9992669753086199E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1316,27 +1373,34 @@
       <c r="D14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <f>SUM(B30+B46)/2</f>
+        <v>-0.12972735268249849</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>6</v>
       </c>
       <c r="B15">
+        <v>-1E-3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15">
         <v>6.9099999999999995E-2</v>
       </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>8</v>
       </c>
       <c r="B16">
-        <v>0.13930000000000001</v>
+        <v>-2.0999999999999999E-3</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
@@ -1344,13 +1408,17 @@
       <c r="D16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <f>SUM(B16+B32+B48)/3</f>
+        <v>2.90393188854495E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>9</v>
       </c>
       <c r="B17">
-        <v>1.8700000000000001E-2</v>
+        <v>-6.9699999999999998E-2</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
@@ -1358,8 +1426,12 @@
       <c r="D17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>-2.9646458786560453E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1373,7 +1445,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1387,7 +1459,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1401,7 +1473,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>4</v>
       </c>
@@ -1415,7 +1487,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>5</v>
       </c>
@@ -1429,7 +1501,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>6</v>
       </c>
@@ -1443,7 +1515,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>8</v>
       </c>
@@ -1457,7 +1529,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>9</v>
       </c>
@@ -1471,7 +1543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1485,7 +1557,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1499,7 +1571,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1513,7 +1585,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>4</v>
       </c>
@@ -1527,7 +1599,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>5</v>
       </c>
@@ -1541,7 +1613,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>6</v>
       </c>
@@ -1555,7 +1627,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>8</v>
       </c>
@@ -1657,14 +1729,14 @@
       <c r="A39">
         <v>6</v>
       </c>
-      <c r="B39">
-        <v>38.383838383838402</v>
+      <c r="B39" t="s">
+        <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D39" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1769,14 +1841,14 @@
       <c r="A47">
         <v>6</v>
       </c>
-      <c r="B47">
-        <v>-0.40000000000000502</v>
+      <c r="B47" t="s">
+        <v>9</v>
       </c>
       <c r="C47" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D47" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>